<commit_message>
Avant ajout d'un random pour le bit genérer
</commit_message>
<xml_diff>
--- a/RRSNRPF.xlsx
+++ b/RRSNRPF.xlsx
@@ -9,13 +9,12 @@
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="26">
   <si>
     <t>nb_user=2</t>
   </si>
@@ -56,18 +55,6 @@
     <t>debit maxSNR</t>
   </si>
   <si>
-    <t>debit PF</t>
-  </si>
-  <si>
-    <t>delais PF</t>
-  </si>
-  <si>
-    <t>delai_proche PF</t>
-  </si>
-  <si>
-    <t>delai_loin PF</t>
-  </si>
-  <si>
     <t>delais RR</t>
   </si>
   <si>
@@ -95,31 +82,16 @@
     <t>nbBitsgenere=250</t>
   </si>
   <si>
-    <t>PDOR RR</t>
+    <t>nb_tours=5000</t>
   </si>
   <si>
-    <t>PDOR maxSNR</t>
+    <t>PDOR</t>
   </si>
   <si>
-    <t>PDOR PF</t>
+    <t>PDORProche</t>
   </si>
   <si>
-    <t>PDORProche RR</t>
-  </si>
-  <si>
-    <t>PDORLoin RR</t>
-  </si>
-  <si>
-    <t>PDORProche maxSNR</t>
-  </si>
-  <si>
-    <t>PDORLoin maxSNR</t>
-  </si>
-  <si>
-    <t>PDORProche PF</t>
-  </si>
-  <si>
-    <t>PDORLoin PF</t>
+    <t>PDORLoin</t>
   </si>
 </sst>
 </file>
@@ -709,14 +681,11 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>debit RR</c:v>
+                  <c:v>debit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>test!$A$2:$A$27</c:f>
@@ -831,10 +800,10 @@
                   <c:v>1016</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1092</c:v>
+                  <c:v>1091</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1167</c:v>
+                  <c:v>1166</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1241</c:v>
@@ -846,34 +815,34 @@
                   <c:v>1390</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1442</c:v>
+                  <c:v>1444</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1446</c:v>
+                  <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1443</c:v>
+                  <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1444</c:v>
+                  <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1444</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1444</c:v>
+                  <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1444</c:v>
+                  <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1446</c:v>
+                  <c:v>1444</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1445</c:v>
@@ -882,7 +851,7 @@
                   <c:v>1445</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1445</c:v>
+                  <c:v>1444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,14 +867,11 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>debit maxSNR</c:v>
+                  <c:v>debit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>test!$K$3:$K$27</c:f>
@@ -958,25 +924,25 @@
                   <c:v>2250</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2345</c:v>
+                  <c:v>2346</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2401</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2446</c:v>
+                  <c:v>2447</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2488</c:v>
+                  <c:v>2487</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2526</c:v>
+                  <c:v>2523</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2554</c:v>
+                  <c:v>2557</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2588</c:v>
+                  <c:v>2589</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2619</c:v>
@@ -1001,14 +967,11 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>debit PF</c:v>
+                  <c:v>debit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>test!$T$3:$T$27</c:f>
@@ -1061,34 +1024,34 @@
                   <c:v>2250</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2366</c:v>
+                  <c:v>2367</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2366</c:v>
+                  <c:v>2367</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2354</c:v>
+                  <c:v>2353</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>2337</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2318</c:v>
+                  <c:v>2317</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2289</c:v>
+                  <c:v>2293</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2267</c:v>
+                  <c:v>2269</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2239</c:v>
+                  <c:v>2240</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>2208</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2177</c:v>
+                  <c:v>2176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,11 +1068,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190509824"/>
-        <c:axId val="190511360"/>
+        <c:axId val="140776576"/>
+        <c:axId val="140778112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190509824"/>
+        <c:axId val="140776576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1081,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190511360"/>
+        <c:crossAx val="140778112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1126,7 +1089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190511360"/>
+        <c:axId val="140778112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,7 +1105,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="190509824"/>
+        <c:crossAx val="140776576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2235,11 +2198,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199629824"/>
-        <c:axId val="199676672"/>
+        <c:axId val="141522432"/>
+        <c:axId val="141523968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199629824"/>
+        <c:axId val="141522432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2211,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199676672"/>
+        <c:crossAx val="141523968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2256,7 +2219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199676672"/>
+        <c:axId val="141523968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2235,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199629824"/>
+        <c:crossAx val="141522432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3365,11 +3328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199701248"/>
-        <c:axId val="199702784"/>
+        <c:axId val="141566720"/>
+        <c:axId val="141568256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199701248"/>
+        <c:axId val="141566720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3378,7 +3341,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199702784"/>
+        <c:crossAx val="141568256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3386,7 +3349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199702784"/>
+        <c:axId val="141568256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3402,7 +3365,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199701248"/>
+        <c:crossAx val="141566720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4495,11 +4458,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199736704"/>
-        <c:axId val="199738496"/>
+        <c:axId val="141619200"/>
+        <c:axId val="141620736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199736704"/>
+        <c:axId val="141619200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4508,7 +4471,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199738496"/>
+        <c:crossAx val="141620736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4516,7 +4479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199738496"/>
+        <c:axId val="141620736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4532,7 +4495,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199736704"/>
+        <c:crossAx val="141619200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5170,11 +5133,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199830144"/>
-        <c:axId val="199856512"/>
+        <c:axId val="141724672"/>
+        <c:axId val="141726464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199830144"/>
+        <c:axId val="141724672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5183,7 +5146,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199856512"/>
+        <c:crossAx val="141726464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5191,7 +5154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199856512"/>
+        <c:axId val="141726464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5207,7 +5170,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199830144"/>
+        <c:crossAx val="141724672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5845,11 +5808,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200218496"/>
-        <c:axId val="200220032"/>
+        <c:axId val="142031104"/>
+        <c:axId val="142032896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200218496"/>
+        <c:axId val="142031104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5858,7 +5821,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200220032"/>
+        <c:crossAx val="142032896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5866,7 +5829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200220032"/>
+        <c:axId val="142032896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5882,7 +5845,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="200218496"/>
+        <c:crossAx val="142031104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6520,11 +6483,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200262784"/>
-        <c:axId val="200264320"/>
+        <c:axId val="142071296"/>
+        <c:axId val="142072832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200262784"/>
+        <c:axId val="142071296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6533,7 +6496,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200264320"/>
+        <c:crossAx val="142072832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6541,7 +6504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200264320"/>
+        <c:axId val="142072832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6557,7 +6520,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="200262784"/>
+        <c:crossAx val="142071296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7195,11 +7158,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="200044928"/>
-        <c:axId val="200046464"/>
+        <c:axId val="141779712"/>
+        <c:axId val="141781248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="200044928"/>
+        <c:axId val="141779712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7208,7 +7171,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200046464"/>
+        <c:crossAx val="141781248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7216,7 +7179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200046464"/>
+        <c:axId val="141781248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7232,7 +7195,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="200044928"/>
+        <c:crossAx val="141779712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7302,7 +7265,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDOR RR</c:v>
+                  <c:v>PDOR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7421,61 +7384,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>69</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>77</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>79</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>81</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>82</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>83</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>84</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>84</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>85</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7491,7 +7454,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDOR maxSNR</c:v>
+                  <c:v>PDOR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7637,34 +7600,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7680,7 +7643,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDOR PF</c:v>
+                  <c:v>PDOR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7826,34 +7789,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>19</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7870,11 +7833,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="160316032"/>
-        <c:axId val="160608640"/>
+        <c:axId val="141819904"/>
+        <c:axId val="141821440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="160316032"/>
+        <c:axId val="141819904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7883,7 +7846,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160608640"/>
+        <c:crossAx val="141821440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7891,7 +7854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="160608640"/>
+        <c:axId val="141821440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7907,7 +7870,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="160316032"/>
+        <c:crossAx val="141819904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7977,7 +7940,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORProche RR</c:v>
+                  <c:v>PDORProche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8111,43 +8074,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>47</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>60</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>68</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>72</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>75</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>78</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>79</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>81</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>82</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>82</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>83</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8163,7 +8126,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORProche maxSNR</c:v>
+                  <c:v>PDORProche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8349,7 +8312,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORProche PF</c:v>
+                  <c:v>PDORProche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8492,34 +8455,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>46</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>67</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>78</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>84</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>85</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>86</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8536,11 +8499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="8419968"/>
-        <c:axId val="8425472"/>
+        <c:axId val="141856768"/>
+        <c:axId val="141858304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8419968"/>
+        <c:axId val="141856768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8549,7 +8512,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8425472"/>
+        <c:crossAx val="141858304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8557,7 +8520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8425472"/>
+        <c:axId val="141858304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8573,7 +8536,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8419968"/>
+        <c:crossAx val="141856768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8648,7 +8611,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORLoin RR</c:v>
+                  <c:v>PDORLoin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8764,61 +8727,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>82</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>83</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>85</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>86</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>87</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>87</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>87</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>88</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>88</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>88</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>88</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>88</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>89</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8834,7 +8797,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORLoin maxSNR</c:v>
+                  <c:v>PDORLoin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8977,34 +8940,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>56</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>62</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>69</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>73</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9020,7 +8983,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PDORLoin PF</c:v>
+                  <c:v>PDORLoin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9207,11 +9170,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126147200"/>
-        <c:axId val="127040896"/>
+        <c:axId val="141872128"/>
+        <c:axId val="141976320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126147200"/>
+        <c:axId val="141872128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9220,7 +9183,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127040896"/>
+        <c:crossAx val="141976320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9228,7 +9191,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127040896"/>
+        <c:axId val="141976320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9244,7 +9207,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="126147200"/>
+        <c:crossAx val="141872128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9314,7 +9277,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delais RR</c:v>
+                  <c:v>delais</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9433,61 +9396,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49</c:v>
+                  <c:v>503</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>85</c:v>
+                  <c:v>857</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>95</c:v>
+                  <c:v>955</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>102</c:v>
+                  <c:v>1018</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>93</c:v>
+                  <c:v>915</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120</c:v>
+                  <c:v>1203</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>146</c:v>
+                  <c:v>1458</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>168</c:v>
+                  <c:v>1681</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>187</c:v>
+                  <c:v>1873</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>204</c:v>
+                  <c:v>2049</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>220</c:v>
+                  <c:v>2203</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>234</c:v>
+                  <c:v>2343</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>246</c:v>
+                  <c:v>2467</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>257</c:v>
+                  <c:v>2583</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>268</c:v>
+                  <c:v>2689</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>277</c:v>
+                  <c:v>2784</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>287</c:v>
+                  <c:v>2873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9503,7 +9466,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delais maxSNR</c:v>
+                  <c:v>delais</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9649,34 +9612,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28</c:v>
+                  <c:v>281</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>52</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>61</c:v>
+                  <c:v>609</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>69</c:v>
+                  <c:v>688</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>75</c:v>
+                  <c:v>752</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>82</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>87</c:v>
+                  <c:v>871</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>92</c:v>
+                  <c:v>923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9692,7 +9655,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delais PF</c:v>
+                  <c:v>delais</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9838,34 +9801,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50</c:v>
+                  <c:v>498</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>64</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>74</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>82</c:v>
+                  <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>85</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>84</c:v>
+                  <c:v>835</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>75</c:v>
+                  <c:v>747</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>60</c:v>
+                  <c:v>602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9882,11 +9845,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="194301952"/>
-        <c:axId val="194303488"/>
+        <c:axId val="140833152"/>
+        <c:axId val="140834688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="194301952"/>
+        <c:axId val="140833152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9895,7 +9858,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194303488"/>
+        <c:crossAx val="140834688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9903,7 +9866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194303488"/>
+        <c:axId val="140834688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9919,7 +9882,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194301952"/>
+        <c:crossAx val="140833152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9989,7 +9952,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_proche RR</c:v>
+                  <c:v>delai_proche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10126,43 +10089,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>76</c:v>
+                  <c:v>759</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>102</c:v>
+                  <c:v>1025</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>126</c:v>
+                  <c:v>1254</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>146</c:v>
+                  <c:v>1465</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>165</c:v>
+                  <c:v>1653</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>182</c:v>
+                  <c:v>1819</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>196</c:v>
+                  <c:v>1968</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>2105</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>223</c:v>
+                  <c:v>2232</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>234</c:v>
+                  <c:v>2346</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>245</c:v>
+                  <c:v>2454</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10178,7 +10141,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_proche maxSNR</c:v>
+                  <c:v>delai_proche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10367,7 +10330,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_proche PF</c:v>
+                  <c:v>delai_proche</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10513,34 +10476,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>61</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>98</c:v>
+                  <c:v>978</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>133</c:v>
+                  <c:v>1311</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>167</c:v>
+                  <c:v>1668</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>206</c:v>
+                  <c:v>2085</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>244</c:v>
+                  <c:v>2462</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>288</c:v>
+                  <c:v>2860</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>322</c:v>
+                  <c:v>3225</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>341</c:v>
+                  <c:v>3567</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10557,11 +10520,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="194386944"/>
-        <c:axId val="194413312"/>
+        <c:axId val="141127040"/>
+        <c:axId val="141137024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="194386944"/>
+        <c:axId val="141127040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10570,7 +10533,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194413312"/>
+        <c:crossAx val="141137024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10578,7 +10541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194413312"/>
+        <c:axId val="141137024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10594,7 +10557,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194386944"/>
+        <c:crossAx val="141127040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10664,7 +10627,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_loin RR</c:v>
+                  <c:v>delai_loin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10783,61 +10746,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34</c:v>
+                  <c:v>329</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89</c:v>
+                  <c:v>913</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>135</c:v>
+                  <c:v>1363</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>171</c:v>
+                  <c:v>1730</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>202</c:v>
+                  <c:v>2025</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>228</c:v>
+                  <c:v>2277</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>247</c:v>
+                  <c:v>2485</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>265</c:v>
+                  <c:v>2661</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>281</c:v>
+                  <c:v>2817</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>296</c:v>
+                  <c:v>2957</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>307</c:v>
+                  <c:v>3075</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>317</c:v>
+                  <c:v>3182</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>327</c:v>
+                  <c:v>3274</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>335</c:v>
+                  <c:v>3361</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>343</c:v>
+                  <c:v>3439</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>350</c:v>
+                  <c:v>3510</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>356</c:v>
+                  <c:v>3579</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>362</c:v>
+                  <c:v>3633</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>368</c:v>
+                  <c:v>3688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10853,7 +10816,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_loin maxSNR</c:v>
+                  <c:v>delai_loin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10999,34 +10962,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54</c:v>
+                  <c:v>541</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>82</c:v>
+                  <c:v>803</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>104</c:v>
+                  <c:v>1044</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>126</c:v>
+                  <c:v>1259</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>148</c:v>
+                  <c:v>1472</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>167</c:v>
+                  <c:v>1665</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>189</c:v>
+                  <c:v>1879</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>211</c:v>
+                  <c:v>2106</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>235</c:v>
+                  <c:v>2368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11042,7 +11005,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>delai_loin PF</c:v>
+                  <c:v>delai_loin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11215,7 +11178,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11232,11 +11195,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="194435328"/>
-        <c:axId val="194441216"/>
+        <c:axId val="141167232"/>
+        <c:axId val="141173120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="194435328"/>
+        <c:axId val="141167232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11245,7 +11208,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="194441216"/>
+        <c:crossAx val="141173120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11253,7 +11216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194441216"/>
+        <c:axId val="141173120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11269,7 +11232,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="194435328"/>
+        <c:crossAx val="141167232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11912,11 +11875,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196901888"/>
-        <c:axId val="196911872"/>
+        <c:axId val="141215616"/>
+        <c:axId val="141217152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196901888"/>
+        <c:axId val="141215616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11925,7 +11888,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196911872"/>
+        <c:crossAx val="141217152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11933,7 +11896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196911872"/>
+        <c:axId val="141217152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11949,7 +11912,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="196901888"/>
+        <c:crossAx val="141215616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12587,11 +12550,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197012096"/>
-        <c:axId val="197017984"/>
+        <c:axId val="141237248"/>
+        <c:axId val="141251328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197012096"/>
+        <c:axId val="141237248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12600,7 +12563,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197017984"/>
+        <c:crossAx val="141251328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12608,7 +12571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197017984"/>
+        <c:axId val="141251328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12624,7 +12587,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="197012096"/>
+        <c:crossAx val="141237248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13267,11 +13230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197044096"/>
-        <c:axId val="197045632"/>
+        <c:axId val="141281536"/>
+        <c:axId val="141283328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197044096"/>
+        <c:axId val="141281536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13280,7 +13243,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197045632"/>
+        <c:crossAx val="141283328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13288,7 +13251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197045632"/>
+        <c:axId val="141283328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13304,7 +13267,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="197044096"/>
+        <c:crossAx val="141281536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13947,11 +13910,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199898240"/>
-        <c:axId val="199899776"/>
+        <c:axId val="141303168"/>
+        <c:axId val="141333632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199898240"/>
+        <c:axId val="141303168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13960,7 +13923,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199899776"/>
+        <c:crossAx val="141333632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13968,7 +13931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199899776"/>
+        <c:axId val="141333632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13984,7 +13947,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199898240"/>
+        <c:crossAx val="141303168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15077,11 +15040,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199946240"/>
-        <c:axId val="199947776"/>
+        <c:axId val="141494528"/>
+        <c:axId val="141504512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199946240"/>
+        <c:axId val="141494528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15090,7 +15053,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199947776"/>
+        <c:crossAx val="141504512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15098,7 +15061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199947776"/>
+        <c:axId val="141504512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15114,7 +15077,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="199946240"/>
+        <c:crossAx val="141494528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16000,8 +15963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16021,7 +15984,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -16033,7 +15996,7 @@
         <v>0</v>
       </c>
       <c r="K1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="L1" t="s">
         <v>2</v>
@@ -16045,7 +16008,7 @@
         <v>0</v>
       </c>
       <c r="T1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="U1" t="s">
         <v>2</v>
@@ -16059,73 +16022,73 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
         <v>4</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>31</v>
-      </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="S2" t="s">
         <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="V2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="W2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Y2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Z2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -16580,22 +16543,22 @@
         <v>1016</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>192</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>34</v>
+        <v>329</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="J9">
         <v>14</v>
@@ -16651,25 +16614,25 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C10">
-        <v>49</v>
+        <v>503</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>89</v>
+        <v>913</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="J10">
         <v>16</v>
@@ -16725,25 +16688,25 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C11">
-        <v>71</v>
+        <v>711</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>135</v>
+        <v>1363</v>
       </c>
       <c r="F11">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="J11">
         <v>18</v>
@@ -16802,22 +16765,22 @@
         <v>1241</v>
       </c>
       <c r="C12">
-        <v>85</v>
+        <v>857</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>171</v>
+        <v>1730</v>
       </c>
       <c r="F12">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="J12">
         <v>20</v>
@@ -16876,22 +16839,22 @@
         <v>1316</v>
       </c>
       <c r="C13">
-        <v>95</v>
+        <v>955</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>202</v>
+        <v>2025</v>
       </c>
       <c r="F13">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="J13">
         <v>22</v>
@@ -16950,22 +16913,22 @@
         <v>1390</v>
       </c>
       <c r="C14">
-        <v>102</v>
+        <v>1018</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>228</v>
+        <v>2277</v>
       </c>
       <c r="F14">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="J14">
         <v>24</v>
@@ -17021,25 +16984,25 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>1442</v>
+        <v>1444</v>
       </c>
       <c r="C15">
-        <v>93</v>
+        <v>915</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="E15">
-        <v>247</v>
+        <v>2485</v>
       </c>
       <c r="F15">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="H15">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="J15">
         <v>26</v>
@@ -17095,25 +17058,25 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="C16">
-        <v>120</v>
+        <v>1203</v>
       </c>
       <c r="D16">
-        <v>46</v>
+        <v>453</v>
       </c>
       <c r="E16">
-        <v>265</v>
+        <v>2661</v>
       </c>
       <c r="F16">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="G16">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="H16">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="J16">
         <v>28</v>
@@ -17172,22 +17135,22 @@
         <v>1445</v>
       </c>
       <c r="C17">
-        <v>146</v>
+        <v>1458</v>
       </c>
       <c r="D17">
-        <v>76</v>
+        <v>759</v>
       </c>
       <c r="E17">
-        <v>281</v>
+        <v>2817</v>
       </c>
       <c r="F17">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="G17">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="H17">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="J17">
         <v>30</v>
@@ -17243,70 +17206,70 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>1443</v>
+        <v>1445</v>
       </c>
       <c r="C18">
-        <v>168</v>
+        <v>1681</v>
       </c>
       <c r="D18">
-        <v>102</v>
+        <v>1025</v>
       </c>
       <c r="E18">
-        <v>296</v>
+        <v>2957</v>
       </c>
       <c r="F18">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="G18">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="H18">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="J18">
         <v>32</v>
       </c>
       <c r="K18">
-        <v>2345</v>
+        <v>2346</v>
       </c>
       <c r="L18">
+        <v>126</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>239</v>
+      </c>
+      <c r="O18">
         <v>13</v>
       </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>25</v>
-      </c>
-      <c r="O18">
-        <v>6</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>12</v>
       </c>
       <c r="S18">
         <v>32</v>
       </c>
       <c r="T18">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="U18">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="V18">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="W18">
         <v>0</v>
       </c>
       <c r="X18">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y18">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="Z18">
         <v>0</v>
@@ -17317,25 +17280,25 @@
         <v>34</v>
       </c>
       <c r="B19">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="C19">
-        <v>187</v>
+        <v>1873</v>
       </c>
       <c r="D19">
-        <v>126</v>
+        <v>1254</v>
       </c>
       <c r="E19">
-        <v>307</v>
+        <v>3075</v>
       </c>
       <c r="F19">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="G19">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="H19">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J19">
         <v>34</v>
@@ -17344,43 +17307,43 @@
         <v>2401</v>
       </c>
       <c r="L19">
-        <v>28</v>
+        <v>281</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <v>54</v>
+        <v>541</v>
       </c>
       <c r="O19">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="S19">
         <v>34</v>
       </c>
       <c r="T19">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="U19">
-        <v>33</v>
+        <v>320</v>
       </c>
       <c r="V19">
-        <v>61</v>
+        <v>600</v>
       </c>
       <c r="W19">
         <v>0</v>
       </c>
       <c r="X19">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="Y19">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -17394,67 +17357,67 @@
         <v>1444</v>
       </c>
       <c r="C20">
-        <v>204</v>
+        <v>2049</v>
       </c>
       <c r="D20">
-        <v>146</v>
+        <v>1465</v>
       </c>
       <c r="E20">
-        <v>317</v>
+        <v>3182</v>
       </c>
       <c r="F20">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="G20">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="H20">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J20">
         <v>36</v>
       </c>
       <c r="K20">
-        <v>2446</v>
+        <v>2447</v>
       </c>
       <c r="L20">
-        <v>41</v>
+        <v>409</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>82</v>
+        <v>803</v>
       </c>
       <c r="O20">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="S20">
         <v>36</v>
       </c>
       <c r="T20">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="U20">
-        <v>50</v>
+        <v>498</v>
       </c>
       <c r="V20">
-        <v>98</v>
+        <v>978</v>
       </c>
       <c r="W20">
         <v>0</v>
       </c>
       <c r="X20">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="Y20">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="Z20">
         <v>0</v>
@@ -17465,49 +17428,49 @@
         <v>38</v>
       </c>
       <c r="B21">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="C21">
-        <v>220</v>
+        <v>2203</v>
       </c>
       <c r="D21">
-        <v>165</v>
+        <v>1653</v>
       </c>
       <c r="E21">
-        <v>327</v>
+        <v>3274</v>
       </c>
       <c r="F21">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="G21">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="H21">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="J21">
         <v>38</v>
       </c>
       <c r="K21">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="L21">
-        <v>52</v>
+        <v>519</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>104</v>
+        <v>1044</v>
       </c>
       <c r="O21">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="P21">
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="S21">
         <v>38</v>
@@ -17516,19 +17479,19 @@
         <v>2337</v>
       </c>
       <c r="U21">
-        <v>64</v>
+        <v>630</v>
       </c>
       <c r="V21">
-        <v>133</v>
+        <v>1311</v>
       </c>
       <c r="W21">
         <v>0</v>
       </c>
       <c r="X21">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="Y21">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -17539,70 +17502,70 @@
         <v>40</v>
       </c>
       <c r="B22">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="C22">
-        <v>234</v>
+        <v>2343</v>
       </c>
       <c r="D22">
-        <v>182</v>
+        <v>1819</v>
       </c>
       <c r="E22">
-        <v>335</v>
+        <v>3361</v>
       </c>
       <c r="F22">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="G22">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="H22">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J22">
         <v>40</v>
       </c>
       <c r="K22">
-        <v>2526</v>
+        <v>2523</v>
       </c>
       <c r="L22">
-        <v>61</v>
+        <v>609</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>126</v>
+        <v>1259</v>
       </c>
       <c r="O22">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="P22">
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="S22">
         <v>40</v>
       </c>
       <c r="T22">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="U22">
-        <v>74</v>
+        <v>739</v>
       </c>
       <c r="V22">
-        <v>167</v>
+        <v>1668</v>
       </c>
       <c r="W22">
         <v>0</v>
       </c>
       <c r="X22">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="Y22">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="Z22">
         <v>0</v>
@@ -17616,67 +17579,67 @@
         <v>1445</v>
       </c>
       <c r="C23">
-        <v>246</v>
+        <v>2467</v>
       </c>
       <c r="D23">
-        <v>196</v>
+        <v>1968</v>
       </c>
       <c r="E23">
-        <v>343</v>
+        <v>3439</v>
       </c>
       <c r="F23">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G23">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="H23">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J23">
         <v>42</v>
       </c>
       <c r="K23">
-        <v>2554</v>
+        <v>2557</v>
       </c>
       <c r="L23">
-        <v>69</v>
+        <v>688</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
-        <v>148</v>
+        <v>1472</v>
       </c>
       <c r="O23">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P23">
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="S23">
         <v>42</v>
       </c>
       <c r="T23">
-        <v>2289</v>
+        <v>2293</v>
       </c>
       <c r="U23">
-        <v>82</v>
+        <v>830</v>
       </c>
       <c r="V23">
-        <v>206</v>
+        <v>2085</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="Y23">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -17687,70 +17650,70 @@
         <v>44</v>
       </c>
       <c r="B24">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="C24">
-        <v>257</v>
+        <v>2583</v>
       </c>
       <c r="D24">
-        <v>210</v>
+        <v>2105</v>
       </c>
       <c r="E24">
-        <v>350</v>
+        <v>3510</v>
       </c>
       <c r="F24">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="G24">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="H24">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J24">
         <v>44</v>
       </c>
       <c r="K24">
-        <v>2588</v>
+        <v>2589</v>
       </c>
       <c r="L24">
-        <v>75</v>
+        <v>752</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
-        <v>167</v>
+        <v>1665</v>
       </c>
       <c r="O24">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="P24">
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="S24">
         <v>44</v>
       </c>
       <c r="T24">
-        <v>2267</v>
+        <v>2269</v>
       </c>
       <c r="U24">
-        <v>85</v>
+        <v>856</v>
       </c>
       <c r="V24">
-        <v>244</v>
+        <v>2462</v>
       </c>
       <c r="W24">
         <v>0</v>
       </c>
       <c r="X24">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="Y24">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -17764,22 +17727,22 @@
         <v>1445</v>
       </c>
       <c r="C25">
-        <v>268</v>
+        <v>2689</v>
       </c>
       <c r="D25">
-        <v>223</v>
+        <v>2232</v>
       </c>
       <c r="E25">
-        <v>356</v>
+        <v>3579</v>
       </c>
       <c r="F25">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G25">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="H25">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J25">
         <v>46</v>
@@ -17788,43 +17751,43 @@
         <v>2619</v>
       </c>
       <c r="L25">
-        <v>82</v>
+        <v>815</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
-        <v>189</v>
+        <v>1879</v>
       </c>
       <c r="O25">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="P25">
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="S25">
         <v>46</v>
       </c>
       <c r="T25">
-        <v>2239</v>
+        <v>2240</v>
       </c>
       <c r="U25">
-        <v>84</v>
+        <v>835</v>
       </c>
       <c r="V25">
-        <v>288</v>
+        <v>2860</v>
       </c>
       <c r="W25">
         <v>1</v>
       </c>
       <c r="X25">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="Y25">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -17838,22 +17801,22 @@
         <v>1445</v>
       </c>
       <c r="C26">
-        <v>277</v>
+        <v>2784</v>
       </c>
       <c r="D26">
-        <v>234</v>
+        <v>2346</v>
       </c>
       <c r="E26">
-        <v>362</v>
+        <v>3633</v>
       </c>
       <c r="F26">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="G26">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="H26">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J26">
         <v>48</v>
@@ -17862,22 +17825,22 @@
         <v>2646</v>
       </c>
       <c r="L26">
-        <v>87</v>
+        <v>871</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
-        <v>211</v>
+        <v>2106</v>
       </c>
       <c r="O26">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="P26">
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="S26">
         <v>48</v>
@@ -17886,19 +17849,19 @@
         <v>2208</v>
       </c>
       <c r="U26">
-        <v>75</v>
+        <v>747</v>
       </c>
       <c r="V26">
-        <v>322</v>
+        <v>3225</v>
       </c>
       <c r="W26">
         <v>1</v>
       </c>
       <c r="X26">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Y26">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -17909,25 +17872,25 @@
         <v>50</v>
       </c>
       <c r="B27">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="C27">
-        <v>287</v>
+        <v>2873</v>
       </c>
       <c r="D27">
-        <v>245</v>
+        <v>2454</v>
       </c>
       <c r="E27">
-        <v>368</v>
+        <v>3688</v>
       </c>
       <c r="F27">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="G27">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="H27">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="J27">
         <v>50</v>
@@ -17936,43 +17899,43 @@
         <v>2673</v>
       </c>
       <c r="L27">
-        <v>92</v>
+        <v>923</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
-        <v>235</v>
+        <v>2368</v>
       </c>
       <c r="O27">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="P27">
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="S27">
         <v>50</v>
       </c>
       <c r="T27">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="U27">
-        <v>60</v>
+        <v>602</v>
       </c>
       <c r="V27">
-        <v>341</v>
+        <v>3567</v>
       </c>
       <c r="W27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Y27">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="Z27">
         <v>0</v>
@@ -17983,7 +17946,7 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
@@ -17995,7 +17958,7 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I62" t="s">
         <v>2</v>
@@ -18007,7 +17970,7 @@
         <v>0</v>
       </c>
       <c r="N62" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O62" t="s">
         <v>2</v>
@@ -18024,13 +17987,13 @@
         <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E63" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -18039,13 +18002,13 @@
         <v>12</v>
       </c>
       <c r="I63" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J63" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K63" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M63" t="s">
         <v>4</v>
@@ -19284,13 +19247,13 @@
         <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D109" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E109" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G109" t="s">
         <v>4</v>
@@ -19299,13 +19262,13 @@
         <v>12</v>
       </c>
       <c r="I109" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J109" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K109" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M109" t="s">
         <v>4</v>
@@ -21681,7 +21644,7 @@
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D180" t="s">
         <v>3</v>
@@ -21693,7 +21656,7 @@
         <v>1</v>
       </c>
       <c r="I180" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J180" t="s">
         <v>9</v>
@@ -21705,7 +21668,7 @@
         <v>1</v>
       </c>
       <c r="O180" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P180" t="s">
         <v>10</v>
@@ -21719,13 +21682,13 @@
         <v>11</v>
       </c>
       <c r="C181" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D181" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E181" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G181" t="s">
         <v>4</v>
@@ -21734,13 +21697,13 @@
         <v>12</v>
       </c>
       <c r="I181" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J181" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K181" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M181" t="s">
         <v>4</v>

</xml_diff>